<commit_message>
agrego FE9252 con canaritos
</commit_message>
<xml_diff>
--- a/Competencia_3/registro_experimentos.xlsx
+++ b/Competencia_3/registro_experimentos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juancho\Desktop\DMEF\labo\Competencia_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ADC6B0C-AC25-42FC-8B3A-12109DF3BD23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9538F4-2859-4D41-ABF5-3E8D81252944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4950" yWindow="2565" windowWidth="21600" windowHeight="11145" xr2:uid="{AF930726-C476-4F77-85C8-6C6A09181C94}"/>
+    <workbookView xWindow="3210" yWindow="2730" windowWidth="21600" windowHeight="11145" xr2:uid="{AF930726-C476-4F77-85C8-6C6A09181C94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>exp</t>
   </si>
@@ -123,6 +123,21 @@
   </si>
   <si>
     <t>FE9251</t>
+  </si>
+  <si>
+    <t>Agrego la tendencia de 12 meses en dataset de train</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>FE9252</t>
+  </si>
+  <si>
+    <t>z925_FE_historia-v1</t>
+  </si>
+  <si>
+    <t>Activo fn CanaritosAsesinos</t>
   </si>
 </sst>
 </file>
@@ -474,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5275DA01-BD44-44B6-92C5-6CAB30176C00}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,6 +502,7 @@
     <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="48.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -520,6 +536,9 @@
       <c r="J1" t="s">
         <v>13</v>
       </c>
+      <c r="K1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -650,11 +669,31 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
       <c r="B6" t="s">
         <v>28</v>
       </c>
       <c r="C6" t="s">
         <v>27</v>
+      </c>
+      <c r="K6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agrego exp TS9313 apilando meses
</commit_message>
<xml_diff>
--- a/Competencia_3/registro_experimentos.xlsx
+++ b/Competencia_3/registro_experimentos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juancho\Desktop\DMEF\labo\Competencia_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9538F4-2859-4D41-ABF5-3E8D81252944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1088AE5E-FA70-4BF1-9AB5-476C0AE5F911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3210" yWindow="2730" windowWidth="21600" windowHeight="11145" xr2:uid="{AF930726-C476-4F77-85C8-6C6A09181C94}"/>
+    <workbookView xWindow="-105" yWindow="2415" windowWidth="21600" windowHeight="11145" xr2:uid="{AF930726-C476-4F77-85C8-6C6A09181C94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,26 +36,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="47">
   <si>
     <t>exp</t>
   </si>
   <si>
-    <t>Input</t>
-  </si>
-  <si>
     <t>TS9320</t>
   </si>
   <si>
-    <t>Output</t>
-  </si>
-  <si>
     <t>HT9421</t>
   </si>
   <si>
-    <t>Script</t>
-  </si>
-  <si>
     <t>z942_HT_lightgbm_under-v1</t>
   </si>
   <si>
@@ -86,9 +77,6 @@
     <t>Semilla</t>
   </si>
   <si>
-    <t>En curso</t>
-  </si>
-  <si>
     <t>TS9310</t>
   </si>
   <si>
@@ -107,9 +95,6 @@
     <t>Aumentando las iteraciones en el script original</t>
   </si>
   <si>
-    <t>FE</t>
-  </si>
-  <si>
     <t>FE9250</t>
   </si>
   <si>
@@ -137,7 +122,61 @@
     <t>z925_FE_historia-v1</t>
   </si>
   <si>
-    <t>Activo fn CanaritosAsesinos</t>
+    <t>Activo fn CanaritosAsesinos y conserva la td de 12 meses</t>
+  </si>
+  <si>
+    <t>HT Script</t>
+  </si>
+  <si>
+    <t>TS Script</t>
+  </si>
+  <si>
+    <t>z931_training_strategy</t>
+  </si>
+  <si>
+    <t>z931_training_strategy_under</t>
+  </si>
+  <si>
+    <t>FE output</t>
+  </si>
+  <si>
+    <t>TS output</t>
+  </si>
+  <si>
+    <t>HT Output</t>
+  </si>
+  <si>
+    <t>TS9311</t>
+  </si>
+  <si>
+    <t>TS9312</t>
+  </si>
+  <si>
+    <t>TS</t>
+  </si>
+  <si>
+    <t>HT9412</t>
+  </si>
+  <si>
+    <t>HT</t>
+  </si>
+  <si>
+    <t>HT9411</t>
+  </si>
+  <si>
+    <t>z931_training_strategy-v0</t>
+  </si>
+  <si>
+    <t>TS9313</t>
+  </si>
+  <si>
+    <t>Apilo 5 meses en train (TS) y agrego la tendencia de 12 meses en dataset de train (FE)</t>
+  </si>
+  <si>
+    <t>Apilo 5 meses en train (TS)</t>
+  </si>
+  <si>
+    <t>TS9314</t>
   </si>
 </sst>
 </file>
@@ -489,211 +528,319 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5275DA01-BD44-44B6-92C5-6CAB30176C00}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="48.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="48.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="F1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" t="s">
-        <v>30</v>
+      <c r="L1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>668111</v>
+      </c>
+      <c r="I2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2">
-        <v>668111</v>
-      </c>
-      <c r="I2">
+      <c r="K2">
         <v>100</v>
       </c>
-      <c r="J2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" t="s">
-        <v>20</v>
+      <c r="L2" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3">
+        <v>102191</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3">
+        <v>50</v>
+      </c>
+      <c r="L3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3">
-        <v>102191</v>
-      </c>
-      <c r="I3">
-        <v>50</v>
-      </c>
-      <c r="J3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" t="s">
-        <v>21</v>
-      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4">
+      <c r="H4">
         <v>102191</v>
       </c>
-      <c r="I4">
+      <c r="I4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4">
         <v>100</v>
       </c>
-      <c r="J4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" t="s">
-        <v>22</v>
+      <c r="L4" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5">
         <v>668111</v>
       </c>
-      <c r="I5">
+      <c r="I5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5">
         <v>50</v>
       </c>
-      <c r="J5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" t="s">
-        <v>20</v>
+      <c r="L5" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
-      </c>
-      <c r="K6" t="s">
-        <v>29</v>
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6">
+        <v>668111</v>
+      </c>
+      <c r="I6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6">
+        <v>50</v>
+      </c>
+      <c r="L6" t="s">
+        <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
         <v>31</v>
       </c>
-      <c r="C7" t="s">
-        <v>32</v>
-      </c>
-      <c r="K7" t="s">
-        <v>33</v>
+      <c r="F7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7">
+        <v>668111</v>
+      </c>
+      <c r="I7" t="s">
+        <v>39</v>
+      </c>
+      <c r="K7">
+        <v>50</v>
+      </c>
+      <c r="L7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remuevo variables azar 942
</commit_message>
<xml_diff>
--- a/Competencia_3/registro_experimentos.xlsx
+++ b/Competencia_3/registro_experimentos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juancho\Desktop\DMEF\labo\Competencia_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1088AE5E-FA70-4BF1-9AB5-476C0AE5F911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F960FB-09ED-45E0-B318-6C834FB52766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="2415" windowWidth="21600" windowHeight="11145" xr2:uid="{AF930726-C476-4F77-85C8-6C6A09181C94}"/>
+    <workbookView xWindow="90" yWindow="90" windowWidth="21600" windowHeight="11145" xr2:uid="{AF930726-C476-4F77-85C8-6C6A09181C94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="51">
   <si>
     <t>exp</t>
   </si>
@@ -110,9 +110,6 @@
     <t>FE9251</t>
   </si>
   <si>
-    <t>Agrego la tendencia de 12 meses en dataset de train</t>
-  </si>
-  <si>
     <t>Descripcion</t>
   </si>
   <si>
@@ -122,9 +119,6 @@
     <t>z925_FE_historia-v1</t>
   </si>
   <si>
-    <t>Activo fn CanaritosAsesinos y conserva la td de 12 meses</t>
-  </si>
-  <si>
     <t>HT Script</t>
   </si>
   <si>
@@ -152,9 +146,6 @@
     <t>TS9312</t>
   </si>
   <si>
-    <t>TS</t>
-  </si>
-  <si>
     <t>HT9412</t>
   </si>
   <si>
@@ -176,7 +167,29 @@
     <t>Apilo 5 meses en train (TS)</t>
   </si>
   <si>
-    <t>TS9314</t>
+    <t>HT9413</t>
+  </si>
+  <si>
+    <t>Agrego la tendencia de 12 meses en dataset de train (FE)</t>
+  </si>
+  <si>
+    <t>Activo fn CanaritosAsesinos y conserva la td de 12 meses (FE)</t>
+  </si>
+  <si>
+    <t>Apilo 5 meses en train (TS) y agrego la tendencia de 12 meses en dataset de train (FE)
+haciendo undersamplig de clase mayoritaria (TS)</t>
+  </si>
+  <si>
+    <t>Cambiando la semilla original del script 942</t>
+  </si>
+  <si>
+    <t>(Variación del exp. 2) Cambiando la semilla original del script 942 y sacando variables de azar</t>
+  </si>
+  <si>
+    <t>z942_HT_lightgbm_under-v2</t>
+  </si>
+  <si>
+    <t>HT9422</t>
   </si>
 </sst>
 </file>
@@ -212,8 +225,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,15 +544,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5275DA01-BD44-44B6-92C5-6CAB30176C00}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="72" customWidth="1"/>
+    <col min="2" max="2" width="84.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.7109375" bestFit="1" customWidth="1"/>
@@ -554,28 +570,28 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
         <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H1" t="s">
         <v>12</v>
       </c>
       <c r="I1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J1" t="s">
         <v>4</v>
@@ -592,7 +608,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
@@ -601,7 +617,7 @@
         <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F2" t="s">
         <v>1</v>
@@ -636,7 +652,7 @@
         <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
         <v>1</v>
@@ -671,7 +687,7 @@
         <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
         <v>1</v>
@@ -706,7 +722,7 @@
         <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -732,7 +748,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
         <v>23</v>
@@ -741,10 +757,10 @@
         <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G6" t="s">
         <v>14</v>
@@ -753,13 +769,13 @@
         <v>668111</v>
       </c>
       <c r="I6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K6">
         <v>50</v>
       </c>
       <c r="L6" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -767,19 +783,19 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
         <v>26</v>
       </c>
-      <c r="D7" t="s">
-        <v>27</v>
-      </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G7" t="s">
         <v>14</v>
@@ -788,13 +804,13 @@
         <v>668111</v>
       </c>
       <c r="I7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="K7">
         <v>50</v>
       </c>
       <c r="L7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -802,7 +818,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
@@ -811,16 +827,25 @@
         <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G8" t="s">
         <v>14</v>
       </c>
+      <c r="H8">
+        <v>668111</v>
+      </c>
+      <c r="I8" t="s">
+        <v>43</v>
+      </c>
+      <c r="K8">
+        <v>50</v>
+      </c>
       <c r="L8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -828,7 +853,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
         <v>23</v>
@@ -837,10 +862,47 @@
         <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>46</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11">
+        <v>668111</v>
+      </c>
+      <c r="I11" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>